<commit_message>
Changes made in admin_msg_dtls
</commit_message>
<xml_diff>
--- a/DB_Design.xlsx
+++ b/DB_Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="103">
   <si>
     <t>PK</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t>UNIQUE_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>OPPONENT_FLAT_DTLS_ID</t>
+  </si>
+  <si>
+    <t>OPPONENT_BUILDING_DTLS_ID</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -448,10 +454,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -748,16 +766,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:L72"/>
+  <dimension ref="B2:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
@@ -768,21 +786,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="J2" s="5" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="J2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="1" t="s">
@@ -1035,11 +1053,11 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="17.25" customHeight="1">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
         <v>8</v>
@@ -1065,11 +1083,11 @@
       <c r="H15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="7"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">
@@ -1117,11 +1135,11 @@
       <c r="D18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
         <v>83</v>
@@ -1321,11 +1339,11 @@
       </c>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="1" t="s">
@@ -1337,27 +1355,27 @@
       <c r="D29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
       <c r="J30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1369,12 +1387,14 @@
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>0</v>
@@ -1398,10 +1418,10 @@
     <row r="32" spans="2:12">
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>25</v>
@@ -1425,10 +1445,10 @@
     <row r="33" spans="2:12">
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>25</v>
@@ -1447,10 +1467,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="15.75">
-      <c r="B34" s="3"/>
+    <row r="34" spans="2:12">
+      <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>4</v>
@@ -1473,10 +1493,10 @@
     <row r="35" spans="2:12" ht="15.75">
       <c r="B35" s="3"/>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
@@ -1496,10 +1516,10 @@
     <row r="36" spans="2:12" ht="15.75">
       <c r="B36" s="3"/>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
@@ -1519,7 +1539,7 @@
     <row r="37" spans="2:12" ht="15.75">
       <c r="B37" s="3"/>
       <c r="C37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>4</v>
@@ -1539,13 +1559,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
-      <c r="B38" s="1"/>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
+    <row r="38" spans="2:12" ht="15.75">
+      <c r="B38" s="3"/>
+      <c r="C38" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="2" t="s">
@@ -1558,7 +1578,7 @@
     <row r="39" spans="2:12">
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>6</v>
@@ -1574,10 +1594,10 @@
     <row r="40" spans="2:12">
       <c r="B40" s="1"/>
       <c r="C40" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="2" t="s">
@@ -1586,16 +1606,16 @@
       <c r="H40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
     </row>
     <row r="41" spans="2:12">
       <c r="B41" s="1"/>
       <c r="C41" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
@@ -1618,6 +1638,13 @@
       </c>
     </row>
     <row r="42" spans="2:12">
+      <c r="B42" s="1"/>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1" t="s">
         <v>95</v>
@@ -1636,16 +1663,11 @@
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7"/>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
         <v>7</v>
@@ -1655,15 +1677,11 @@
       </c>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="7"/>
       <c r="F45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1683,10 +1701,10 @@
     </row>
     <row r="46" spans="2:12">
       <c r="B46" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>1</v>
@@ -1713,7 +1731,7 @@
         <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>1</v>
@@ -1729,12 +1747,14 @@
       </c>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C48" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>25</v>
@@ -1746,13 +1766,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:12">
+    <row r="49" spans="2:13">
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
@@ -1761,16 +1781,16 @@
       <c r="H49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-    </row>
-    <row r="50" spans="2:12" ht="15.75">
-      <c r="B50" s="3"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="2:13">
+      <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>4</v>
@@ -1794,13 +1814,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="15.75">
+    <row r="51" spans="2:13" ht="15.75">
       <c r="B51" s="3"/>
       <c r="C51" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -1817,13 +1837,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:12" ht="15.75">
+    <row r="52" spans="2:13" ht="15.75">
       <c r="B52" s="3"/>
       <c r="C52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
@@ -1840,10 +1860,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="15.75">
+    <row r="53" spans="2:13" ht="15.75">
       <c r="B53" s="3"/>
       <c r="C53" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>4</v>
@@ -1863,13 +1883,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="15.75">
-      <c r="B54" s="1"/>
-      <c r="C54" s="2" t="s">
-        <v>5</v>
+    <row r="54" spans="2:13" ht="15.75">
+      <c r="B54" s="3"/>
+      <c r="C54" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="2" t="s">
@@ -1886,10 +1906,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:12">
+    <row r="55" spans="2:13">
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>6</v>
@@ -1911,13 +1931,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:12">
+    <row r="56" spans="2:13">
       <c r="B56" s="1"/>
       <c r="C56" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="2" t="s">
@@ -1934,10 +1954,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="2:12">
+    <row r="57" spans="2:13">
       <c r="B57" s="1"/>
       <c r="C57" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>9</v>
@@ -1957,7 +1977,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:12">
+    <row r="58" spans="2:13">
+      <c r="B58" s="1"/>
+      <c r="C58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F58" s="1"/>
       <c r="G58" s="2" t="s">
         <v>5</v>
@@ -1973,7 +2000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:12">
+    <row r="59" spans="2:13">
       <c r="F59" s="1"/>
       <c r="G59" s="2" t="s">
         <v>7</v>
@@ -1982,12 +2009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:12">
-      <c r="B60" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
+    <row r="60" spans="2:13">
       <c r="F60" s="1"/>
       <c r="G60" s="2" t="s">
         <v>8</v>
@@ -1996,16 +2018,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="2:12">
-      <c r="B61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="61" spans="2:13">
+      <c r="B61" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="10"/>
       <c r="F61" s="1"/>
       <c r="G61" s="2" t="s">
         <v>10</v>
@@ -2014,45 +2032,48 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="2:12">
-      <c r="B62" s="1"/>
+    <row r="62" spans="2:13">
+      <c r="B62" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12">
+        <v>1</v>
+      </c>
+      <c r="M62" s="13"/>
+    </row>
+    <row r="63" spans="2:13">
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="2:12">
+    <row r="64" spans="2:13">
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G64" s="6"/>
-      <c r="H64" s="7"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>0</v>
@@ -2067,7 +2088,7 @@
     <row r="66" spans="2:8">
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>19</v>
@@ -2085,10 +2106,10 @@
     <row r="67" spans="2:8">
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
@@ -2101,10 +2122,10 @@
     <row r="68" spans="2:8" ht="15.75">
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3" t="s">
@@ -2116,11 +2137,11 @@
     </row>
     <row r="69" spans="2:8" ht="15.75">
       <c r="B69" s="1"/>
-      <c r="C69" s="2" t="s">
-        <v>5</v>
+      <c r="C69" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="2" t="s">
@@ -2133,7 +2154,7 @@
     <row r="70" spans="2:8">
       <c r="B70" s="1"/>
       <c r="C70" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>6</v>
@@ -2149,10 +2170,10 @@
     <row r="71" spans="2:8">
       <c r="B71" s="1"/>
       <c r="C71" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="2" t="s">
@@ -2165,7 +2186,7 @@
     <row r="72" spans="2:8">
       <c r="B72" s="1"/>
       <c r="C72" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>9</v>
@@ -2178,23 +2199,31 @@
         <v>9</v>
       </c>
     </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="1"/>
+      <c r="C73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="F64:H64"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="F44:H44"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B60:D60"/>
     <mergeCell ref="J40:L40"/>
     <mergeCell ref="J29:L29"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="J49:L49"/>
+    <mergeCell ref="B61:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>